<commit_message>
removed dependence on membraneEOS for setup files
</commit_message>
<xml_diff>
--- a/test/template_results/TPBO-0.75_CO2_27C_saved_template.xlsx
+++ b/test/template_results/TPBO-0.75_CO2_27C_saved_template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>Overall Properties</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Dual Mode Pred Err (CC/CC)</t>
+  </si>
+  <si>
+    <t>CO2</t>
   </si>
   <si>
     <t>TPBO-0.75</t>
@@ -565,6 +568,9 @@
       <c r="A2" t="s">
         <v>13</v>
       </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -719,7 +725,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
possible circumvent missing issue while saving
</commit_message>
<xml_diff>
--- a/test/template_results/TPBO-0.75_CO2_27C_saved_template.xlsx
+++ b/test/template_results/TPBO-0.75_CO2_27C_saved_template.xlsx
@@ -604,7 +604,7 @@
         <v>0.228</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -636,7 +636,7 @@
         <v>72.83494</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -668,7 +668,7 @@
         <v>304.18</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -688,7 +688,7 @@
         <v>44.01</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -717,7 +717,7 @@
         <v>0.13399839</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -734,10 +734,10 @@
         <v>10</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9" spans="1:17">

</xml_diff>